<commit_message>
Update threat model report and data-flow diagram by Threagile
</commit_message>
<xml_diff>
--- a/threagile/output/tags.xlsx
+++ b/threagile/output/tags.xlsx
@@ -7,43 +7,79 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Model Stub" sheetId="2" r:id="rId4"/>
+    <sheet name="SAPL.io" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Element</t>
   </si>
   <si>
-    <t>some-other-tag</t>
-  </si>
-  <si>
-    <t>some-tag</t>
-  </si>
-  <si>
-    <t>Some Other Technical Asset</t>
+    <t>sapl-jwt</t>
+  </si>
+  <si>
+    <t>sapl-spring-pdp-embedded</t>
+  </si>
+  <si>
+    <t>sapl-webflux-endpoint</t>
+  </si>
+  <si>
+    <t>spring-boot</t>
+  </si>
+  <si>
+    <t>spring-security</t>
+  </si>
+  <si>
+    <t>windows-server</t>
+  </si>
+  <si>
+    <t>Customer Web Client</t>
+  </si>
+  <si>
+    <t>Customer Traffic</t>
+  </si>
+  <si>
+    <t>Policy Fileserver</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Some Technical Asset</t>
-  </si>
-  <si>
-    <t>Some Traffic</t>
-  </si>
-  <si>
-    <t>Some Data Asset</t>
-  </si>
-  <si>
-    <t>Some Trust Boundary</t>
-  </si>
-  <si>
-    <t>Some Shared Runtime</t>
+    <t>SAPL MVC</t>
+  </si>
+  <si>
+    <t>SAPL Server LT Traffic</t>
+  </si>
+  <si>
+    <t>SAPL Server LT</t>
+  </si>
+  <si>
+    <t>Policy Filesystem Access</t>
+  </si>
+  <si>
+    <t>Access-Decision</t>
+  </si>
+  <si>
+    <t>Access-Request</t>
+  </si>
+  <si>
+    <t>Patient Data</t>
+  </si>
+  <si>
+    <t>Policies</t>
+  </si>
+  <si>
+    <t>File-Server Network</t>
+  </si>
+  <si>
+    <t>SAPL-Server DMZ</t>
+  </si>
+  <si>
+    <t>Web DMZ</t>
   </si>
 </sst>
 </file>
@@ -396,7 +432,7 @@
   </sheetViews>
   <cols>
     <col customWidth="true" max="1" min="1" width="60"/>
-    <col customWidth="true" max="3" min="2" width="35"/>
+    <col customWidth="true" max="7" min="2" width="35"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -409,56 +445,186 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>
@@ -467,7 +633,7 @@
     <oddFooter>&amp;C&amp;F</oddFooter>
     <evenHeader>&amp;L&amp;P</evenHeader>
     <evenFooter>&amp;L&amp;D&amp;R&amp;T</evenFooter>
-    <firstHeader>&amp;Tag Matrix &amp;"-,Model Stub"Bold&amp;"-,Regular"Summary+000A&amp;D</firstHeader>
+    <firstHeader>&amp;Tag Matrix &amp;"-,SAPL.io"Bold&amp;"-,Regular"Summary+000A&amp;D</firstHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>